<commit_message>
Changed layout of a few cells
</commit_message>
<xml_diff>
--- a/Results of forms/Time results.xlsx
+++ b/Results of forms/Time results.xlsx
@@ -158,7 +158,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -186,25 +186,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -216,8 +209,14 @@
     <xf numFmtId="1" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="27">
+  <cellStyles count="29">
     <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -231,6 +230,7 @@
     <cellStyle name="Gevolgde hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -244,6 +244,7 @@
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normaal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -573,10 +574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -587,485 +588,482 @@
     <col min="9" max="9" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:10">
+      <c r="A1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6" t="s">
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="10" t="s">
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="9" customFormat="1">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="8" t="s">
+    <row r="2" spans="1:10" s="6" customFormat="1">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="11"/>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="4">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="I2" s="8"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>0.1125</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>3.4722222222222224E-2</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>0.16458333333333333</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <v>0.16527777777777777</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="4">
         <v>7.5694444444444439E-2</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="4">
         <v>7.9166666666666663E-2</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="4">
+      <c r="I3" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>0.10694444444444444</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>5.8333333333333327E-2</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>0.17986111111111111</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>7.7083333333333337E-2</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="4">
         <v>7.9166666666666663E-2</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="4">
         <v>4.7916666666666663E-2</v>
       </c>
-      <c r="I4" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="4">
+      <c r="I4" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="3">
         <v>3</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>8.4722222222222213E-2</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>0.22152777777777777</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>9.8611111111111108E-2</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>6.3194444444444442E-2</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="4">
         <v>0.11666666666666665</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="4">
         <v>8.6111111111111124E-2</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="4" t="s">
         <v>2</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="4">
+    <row r="6" spans="1:10">
+      <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>0.12152777777777778</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>4.0972222222222222E-2</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>7.5694444444444439E-2</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>0.10347222222222223</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="4">
         <v>0.14722222222222223</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="4">
         <v>6.5277777777777782E-2</v>
       </c>
-      <c r="I6" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" s="4">
+      <c r="I6" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>0.47430555555555554</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>0.24374999999999999</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <v>0.10486111111111111</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <v>5.9722222222222225E-2</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="4">
         <v>8.1250000000000003E-2</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="4">
         <v>5.4166666666666669E-2</v>
       </c>
-      <c r="I7" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" s="4">
+      <c r="I7" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="3">
         <v>6</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <v>0.10277777777777779</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>0.10347222222222223</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <v>8.1250000000000003E-2</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <v>0.12291666666666667</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="4">
         <v>0.15347222222222223</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="4">
         <v>0.10277777777777779</v>
       </c>
-      <c r="I8" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9" s="4">
+      <c r="I8" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="3">
         <v>7</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>0.15625</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="9">
         <v>0.36249999999999999</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="5">
+      <c r="E9" s="9"/>
+      <c r="F9" s="4">
         <v>4.9305555555555554E-2</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="9">
         <v>0.23263888888888887</v>
       </c>
-      <c r="H9" s="7"/>
-      <c r="I9" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="4">
+      <c r="H9" s="9"/>
+      <c r="I9" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="3">
         <v>8</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>0.24722222222222223</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>0.28750000000000003</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <v>0.11666666666666665</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <v>7.9861111111111105E-2</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="4">
         <v>8.7500000000000008E-2</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10" s="4">
         <v>0.11388888888888889</v>
       </c>
-      <c r="I10" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="A11" s="4">
+      <c r="I10" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="3">
         <v>9</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="4">
         <v>6.0416666666666667E-2</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <v>9.9999999999999992E-2</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="4">
         <v>7.013888888888889E-2</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <v>0.14166666666666666</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="4">
         <v>9.8611111111111108E-2</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11" s="4">
         <v>9.375E-2</v>
       </c>
-      <c r="I11" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="A12" s="4">
+      <c r="I11" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="3">
         <v>10</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="4">
         <v>7.5694444444444439E-2</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4">
         <v>9.0972222222222218E-2</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="4">
         <v>6.1111111111111116E-2</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="4">
         <v>0.11527777777777777</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="4">
         <v>0.14722222222222223</v>
       </c>
-      <c r="H12" s="5">
+      <c r="H12" s="4">
         <v>7.3611111111111113E-2</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="I12" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="4">
+    <row r="13" spans="1:10">
+      <c r="A13" s="3">
         <v>11</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="9">
         <v>0.25625000000000003</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7" t="s">
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="4">
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="3">
         <v>12</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="9">
         <v>0.26944444444444443</v>
       </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7">
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9">
         <v>0.26597222222222222</v>
       </c>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="K14" s="3"/>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="A15" s="4">
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="3">
         <v>13</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="4">
         <v>0.1451388888888889</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="4">
         <v>7.9166666666666663E-2</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="4">
         <v>7.5694444444444439E-2</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="4">
         <v>0.12569444444444444</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G15" s="4">
         <v>5.486111111111111E-2</v>
       </c>
-      <c r="H15" s="5">
+      <c r="H15" s="4">
         <v>0.15069444444444444</v>
       </c>
-      <c r="I15" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="K15" s="4"/>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="A16" s="4">
+      <c r="I15" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="3">
         <v>14</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="9">
         <v>0.47916666666666669</v>
       </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7" t="s">
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="5" t="s">
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="K16" s="5"/>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="4">
+      <c r="A17" s="3">
         <v>15</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="4">
         <v>0.15069444444444444</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="4">
         <v>6.7361111111111108E-2</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="4">
         <v>0.21597222222222223</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17" s="4">
         <v>0.12152777777777778</v>
       </c>
-      <c r="G17" s="5">
+      <c r="G17" s="4">
         <v>0.15625</v>
       </c>
-      <c r="H17" s="5">
+      <c r="H17" s="4">
         <v>9.3055555555555558E-2</v>
       </c>
-      <c r="I17" s="5" t="s">
+      <c r="I17" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="4">
+      <c r="A18" s="3">
         <v>16</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="4">
         <v>9.9999999999999992E-2</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="4">
         <v>0.10416666666666667</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="4">
         <v>0.1076388888888889</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F18" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="5" t="s">
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="4" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1074,12 +1072,6 @@
     <sortCondition ref="A2"/>
   </sortState>
   <mergeCells count="14">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="F13:H13"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="C16:E16"/>
     <mergeCell ref="F16:H16"/>
@@ -1088,6 +1080,12 @@
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="C14:E14"/>
     <mergeCell ref="F14:H14"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="F13:H13"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>